<commit_message>
art + ui \= world
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>grass, cleanup, fps</t>
+  </si>
+  <si>
+    <t>water dropping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">art overhaul + ui, world beginnings </t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +512,7 @@
       </c>
       <c r="F1" s="10">
         <f>SUM(C2:C27)</f>
-        <v>17.399999999999999</v>
+        <v>22.799999999999997</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -603,6 +609,12 @@
       <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -612,6 +624,12 @@
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -662,7 +680,7 @@
       </c>
       <c r="F13">
         <f>SUM(C7:C13)</f>
-        <v>0</v>
+        <v>5.3999999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>